<commit_message>
added unit tests for the present sprint overview use case.
</commit_message>
<xml_diff>
--- a/doc/use cases/update-vacation-hours/update-vacation-hours-decision-table.xlsx
+++ b/doc/use cases/update-vacation-hours/update-vacation-hours-decision-table.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects.pet\VeloCity\repo\doc\use cases\update-vacation-hours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A055D826-AF6F-4A47-AA9C-B4E4D73EFA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA09EE5-67E7-4FB8-AB7E-37491EA82727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
   <si>
     <t>any</t>
   </si>
@@ -75,9 +74,6 @@
     <t>employment</t>
   </si>
   <si>
-    <t>vacation hours are not changed for specified date and TeamMemberVacationChangedEvent is NOT published</t>
-  </si>
-  <si>
     <t>vacation hours are updated for specified date and TeamMemberVacationChangedEvent is published</t>
   </si>
   <si>
@@ -87,9 +83,6 @@
     <t>exists for date</t>
   </si>
   <si>
-    <t>not zero</t>
-  </si>
-  <si>
     <t>vacation hours remains zero for specified date</t>
   </si>
   <si>
@@ -97,12 +90,6 @@
   </si>
   <si>
     <t>does not exist for date</t>
-  </si>
-  <si>
-    <t>not zero (equal to requested)</t>
-  </si>
-  <si>
-    <t>not zero (different than requested)</t>
   </si>
   <si>
     <t>positive (other)</t>
@@ -205,7 +192,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -215,25 +202,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -552,208 +536,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C7C8EE-3D34-4140-B67F-232CA24D32CB}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
-    <col min="10" max="15" width="22.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="39.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65255CD2-7F83-4308-8D8B-87AD40DBECF2}">
   <dimension ref="A1:E20"/>
   <sheetViews>
@@ -788,48 +570,48 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="7"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="9"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -840,20 +622,20 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
@@ -861,82 +643,82 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7" t="s">
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -947,20 +729,20 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="9"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="9"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
@@ -968,38 +750,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6" t="s">
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7" t="s">
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7" t="s">
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1008,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>0</v>
@@ -1022,15 +804,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B11:B19"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B11:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>